<commit_message>
Issue #24 updated Company Details.xlxs
</commit_message>
<xml_diff>
--- a/Project Code/Data/List_of_NSU_graduates/Company Details.xlsx
+++ b/Project Code/Data/List_of_NSU_graduates/Company Details.xlsx
@@ -461,7 +461,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +490,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -503,7 +503,7 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhancement #24  : Collected company details
</commit_message>
<xml_diff>
--- a/Project Code/Data/List_of_NSU_graduates/Company Details.xlsx
+++ b/Project Code/Data/List_of_NSU_graduates/Company Details.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>Company Name</t>
   </si>
@@ -106,6 +106,571 @@
   </si>
   <si>
     <t>0155 015 4444</t>
+  </si>
+  <si>
+    <t>Tiger IT Bangladesh Limited</t>
+  </si>
+  <si>
+    <t>House 21, Road 28, Block-K, Banani Model Town
+Dhaka, 1213</t>
+  </si>
+  <si>
+    <t>http://www.tigerit.com</t>
+  </si>
+  <si>
+    <t>https://brainstation-23.com/</t>
+  </si>
+  <si>
+    <t>Brain Station 23</t>
+  </si>
+  <si>
+    <t>8th floor, Plot-02, Amtoli, Bir Uttam Ak Khandaker Rd, Dhaka 1212</t>
+  </si>
+  <si>
+    <t>DataSoft Systems Bangladesh Limited</t>
+  </si>
+  <si>
+    <t>Rupayan Shelford (20th Floor), 23/6, Mirpur Road, Shyamoli, Dhaka-1207, Bangladesh.</t>
+  </si>
+  <si>
+    <t>info@datasoft-bd.com</t>
+  </si>
+  <si>
+    <t>http://datasoft-bd.com</t>
+  </si>
+  <si>
+    <t>IBCS-PRIMAX Software(Bangladesh) Limited</t>
+  </si>
+  <si>
+    <t>House # 51, Road # 10A, Dhanmondi R/A,
+Dhaka-1209, Bangladesh</t>
+  </si>
+  <si>
+    <t>info@ibcs-primax.com</t>
+  </si>
+  <si>
+    <t>http://www.ibcs-primax.com</t>
+  </si>
+  <si>
+    <t>Invento Bangladesh</t>
+  </si>
+  <si>
+    <t>House no: 484 (4th Floor) , Road no 32, Mohakhali DOHS, Dhaka 1206</t>
+  </si>
+  <si>
+    <t>880 1682 244 434</t>
+  </si>
+  <si>
+    <t>hello@invento.com.bd</t>
+  </si>
+  <si>
+    <t>www.invento.com.bd</t>
+  </si>
+  <si>
+    <t>PRAN-RFL GROUP LTD</t>
+  </si>
+  <si>
+    <t>PRAN-RFL Centre
+105, Progoti Sarani Middle Badda
+Dhaka 1212, Bangladesh</t>
+  </si>
+  <si>
+    <t>09613-737777</t>
+  </si>
+  <si>
+    <t>https://www.pranfoods.net/</t>
+  </si>
+  <si>
+    <t>crd@prangroup.com</t>
+  </si>
+  <si>
+    <t>https://www.nestle.com.bd/</t>
+  </si>
+  <si>
+    <t>227/A Bir Uttam Mir Showkat Ali Road, 1208 Tejgaon Farm, Dhaka, Bangladesh</t>
+  </si>
+  <si>
+    <t>Nestlé Bangladesh Limited</t>
+  </si>
+  <si>
+    <t>https://www.sc.com/bd/</t>
+  </si>
+  <si>
+    <t>88 02 55669900</t>
+  </si>
+  <si>
+    <t>customer.enquiries@sc.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Chartered Bank,
+67 Gulshan Avenue, Gulshan
+Dhaka 1212, Bangladesh </t>
+  </si>
+  <si>
+    <t>Standard Chartered | Bangladesh</t>
+  </si>
+  <si>
+    <t>71, Purana Paltan Lane, Dhaka</t>
+  </si>
+  <si>
+    <t>Dhaka Bank Limited</t>
+  </si>
+  <si>
+    <t>info@dhakabank.com.bd</t>
+  </si>
+  <si>
+    <t>5831 4624-8</t>
+  </si>
+  <si>
+    <t>https://dhakabankltd.com</t>
+  </si>
+  <si>
+    <t>https://www.thecitybank.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">136, Gulshan Avenue, Gulshan-2
+Dhaka-1212, Bangladesh </t>
+  </si>
+  <si>
+    <t>City Bank Ltd</t>
+  </si>
+  <si>
+    <t>info@thecitybank.com.bd</t>
+  </si>
+  <si>
+    <t>Plot - CWS- (A)-1
+Road No - 34
+Gulshan Avenue, Dhaka-1212</t>
+  </si>
+  <si>
+    <t>United Commercial Bank Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> info@ucb.com.bd</t>
+  </si>
+  <si>
+    <t>88-02-55668070</t>
+  </si>
+  <si>
+    <t>https://www.ucb.com.bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern Bank Ltd.
+100 Gulshan Avenue
+Dhaka-1212,
+Bangladesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> info@ebl.com.bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88 09666777325 </t>
+  </si>
+  <si>
+    <t>https://www.ebl.com.bd</t>
+  </si>
+  <si>
+    <t>Eastern Bank Ltd</t>
+  </si>
+  <si>
+    <t>Anik Tower, 220/B Bir Uttam Mir Shawkat Sarak, Dhaka 1208</t>
+  </si>
+  <si>
+    <t>enquiry@bracbank.com</t>
+  </si>
+  <si>
+    <t>https://www.bracbank.com</t>
+  </si>
+  <si>
+    <t>BRAC Bank Limited</t>
+  </si>
+  <si>
+    <t>Islami Bank Tower
+40, Dilkusha C/A
+Dhaka - 1000
+Bangladesh</t>
+  </si>
+  <si>
+    <t>Islami Bank Bangladesh Limited</t>
+  </si>
+  <si>
+    <t>https://www.islamibankbd.com</t>
+  </si>
+  <si>
+    <t>info@islamibankbd.com</t>
+  </si>
+  <si>
+    <t>Safura Tower (Level 11)20 Kemal Ataturk Avenue, Banani, Dhaka</t>
+  </si>
+  <si>
+    <t>LankaBangla Finance</t>
+  </si>
+  <si>
+    <t>info@lankabangla.com</t>
+  </si>
+  <si>
+    <t>(+88 02) 9883701-10</t>
+  </si>
+  <si>
+    <t>https://www.lankabangla.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unilever Bangladesh Ltd 
+ZN Tower, Plot# 02 
+Road # 08, Gulshan - 1 
+Dhaka - 1212. 
+Unilever Bangladesh   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">880 2 988 8452  </t>
+  </si>
+  <si>
+    <t>careline.bd@unilever.com</t>
+  </si>
+  <si>
+    <t>www.unilever.com.bd</t>
+  </si>
+  <si>
+    <t>Uniliver Bangladesh</t>
+  </si>
+  <si>
+    <t>Reckitt Benckiser Bangladesh ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot 2 (B)
+Block SE (C), Road 138
+Gulshan-1, Dhaka-1212
+Bangladesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">88 02 988 7209 </t>
+  </si>
+  <si>
+    <t>www.rb.com</t>
+  </si>
+  <si>
+    <t>House 2A, Road 138
+Gulshan 1,Dhaka 1212
+Bangladesh</t>
+  </si>
+  <si>
+    <t>gsk.bangladesh-info@gsk.com</t>
+  </si>
+  <si>
+    <t>88 02 985 8870</t>
+  </si>
+  <si>
+    <t>https://www.gsk.com/en-gb/contact-us/worldwide/bangladesh/</t>
+  </si>
+  <si>
+    <t>GlaxoSmithKline plc</t>
+  </si>
+  <si>
+    <t>SQUARE Centre 48, Mohakhali C/A Dhaka 1212, Bangladesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88-02-8833047-56 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@squaregroup.com </t>
+  </si>
+  <si>
+    <t>https://www.squaregroup.com/</t>
+  </si>
+  <si>
+    <t>SQUARE GROUP</t>
+  </si>
+  <si>
+    <t>http://www.squarepharma.com.bd/</t>
+  </si>
+  <si>
+    <t>48, Mohakhali C/A
+Dhaka 1212,
+Bangladesh.</t>
+  </si>
+  <si>
+    <t>02-9859007</t>
+  </si>
+  <si>
+    <t>http://www.squarepharma.com.bd/contact-us.php</t>
+  </si>
+  <si>
+    <t>Square Pharmaceuticals Ltd</t>
+  </si>
+  <si>
+    <t>Square Toiletries Limited</t>
+  </si>
+  <si>
+    <t>Rupayan Centre [12th Floor]
+72, Mohakhali C/A, Dhaka-1212</t>
+  </si>
+  <si>
+    <t>880-2-9841531-40, Ext: 213</t>
+  </si>
+  <si>
+    <t>http://squaretoiletries.com</t>
+  </si>
+  <si>
+    <t>sfblcareline@squaregroup.com</t>
+  </si>
+  <si>
+    <t>09-612-111-333</t>
+  </si>
+  <si>
+    <t>http://www.sfbl.com.bd</t>
+  </si>
+  <si>
+    <t>Square Food &amp; Beverage Limited
+Square Centre (6th Floor)
+Corporate Head Quarter.
+48, Mohakhali CA, Dhaka-1212.</t>
+  </si>
+  <si>
+    <t>Square Food &amp; Beverage Limited</t>
+  </si>
+  <si>
+    <t>Square Center (11th Floor),
+48, Mohakhali C/A, Dhaka-1212, Bangladesh.</t>
+  </si>
+  <si>
+    <t>Square Informatix Limited</t>
+  </si>
+  <si>
+    <t>info@squarecloud.net</t>
+  </si>
+  <si>
+    <t>09613707070 - Ext 2057</t>
+  </si>
+  <si>
+    <t>https://www.squarecloud.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> H.No 19, R/A, Rd No. 7, Dhaka 1205</t>
+  </si>
+  <si>
+    <t>info@bpl.net</t>
+  </si>
+  <si>
+    <t>880-2-58611001-7</t>
+  </si>
+  <si>
+    <t>https://www.beximcopharma.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beximco Pharmaceuticals Ltd.
+</t>
+  </si>
+  <si>
+    <t>http://www.meghnacement.com/</t>
+  </si>
+  <si>
+    <t>Bashundhara Industrial Head Quarters, Plot-3,
+Block-G (Umme Kulsum Road), Bashundhara R/A, Dhaka - 1229.</t>
+  </si>
+  <si>
+    <t>88 02 8431024-8,</t>
+  </si>
+  <si>
+    <t>info.mcmlfactory@bg.com.bd</t>
+  </si>
+  <si>
+    <t>Meghna Cement.</t>
+  </si>
+  <si>
+    <t>http://www.bashundharafood.com/</t>
+  </si>
+  <si>
+    <t>Bashundhara Industrial Head Quarters 2, Plot#56/A, Block#C, 2nd Avenue, Bashundhara R/A, Dhaka-1229, Bangladesh</t>
+  </si>
+  <si>
+    <t>88-02-8431256-8</t>
+  </si>
+  <si>
+    <t>bfbil@bg.com.bd</t>
+  </si>
+  <si>
+    <t>Bashundhara Food &amp; Beverage Industries Ltd.</t>
+  </si>
+  <si>
+    <t>bashundhara.cement@bg.com.bd</t>
+  </si>
+  <si>
+    <t>Plot# 3, Block# G, Umme Kulsum Road, Bashundhara R/A, Dhaka-1229</t>
+  </si>
+  <si>
+    <t>880 2 8431024-8</t>
+  </si>
+  <si>
+    <t>http://www.bashundharacement.com/</t>
+  </si>
+  <si>
+    <t>Bashundhara Industrial Complex Limited</t>
+  </si>
+  <si>
+    <t>http://www.bashundharapapermills.com/</t>
+  </si>
+  <si>
+    <t>88 02 8432289-93</t>
+  </si>
+  <si>
+    <t>info.paper@bg.com.bd</t>
+  </si>
+  <si>
+    <t>Bashundhara Industrial Headquarters- 2, Plot# 56/A, Block# C, Umme Kulsum Road, Bashundhara R/A, Dhaka-1229, Bangladesh</t>
+  </si>
+  <si>
+    <t>Bashundhara Paper Mills Limited</t>
+  </si>
+  <si>
+    <t>https://www.haquegroupbd.com/</t>
+  </si>
+  <si>
+    <t>Ibrahim Chamber
+95, Motijheel C/A (2nd &amp; 3rd Floor)
+Dhaka - 1000, Bangladesh.</t>
+  </si>
+  <si>
+    <t>880-2-9554670</t>
+  </si>
+  <si>
+    <t>info@haquegroupbd.com</t>
+  </si>
+  <si>
+    <t>haque group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOUSE # 14, ROAD # 16/A (2nd Floor) GULSHAN-1, Dhaka-1212, Bangladesh </t>
+  </si>
+  <si>
+    <t>Cocola Food Products Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88-01711-000000 </t>
+  </si>
+  <si>
+    <t>http://www.cocolafood.net</t>
+  </si>
+  <si>
+    <t>Nabisco Biscuit and Bread Factory Ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77, Shaid Tajuddin Ahmed Sarani, Dhaka-1208, Bangladesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">01741-116813 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Romania Food &amp; Beverage Ltd.
+</t>
+  </si>
+  <si>
+    <t>nabisco077@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+http://romania.com.bd/
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House, 75, Gulshan Avenue, Road-30, Gulshan-1, Dhaka-1212, Bangladesh, </t>
+  </si>
+  <si>
+    <t>88-02-9888248</t>
+  </si>
+  <si>
+    <t>75 Gulshan Avenue
+Gulshan 1, Dhaka 1212
+Bangladesh.</t>
+  </si>
+  <si>
+    <t>Bengal Group of Industries</t>
+  </si>
+  <si>
+    <t>info@bengal.com.bd</t>
+  </si>
+  <si>
+    <t>880-2-9888248</t>
+  </si>
+  <si>
+    <t>https://www.bengalgroup.com</t>
+  </si>
+  <si>
+    <t>https://transcomdigital.com/</t>
+  </si>
+  <si>
+    <t>estore@transcomdigital.com</t>
+  </si>
+  <si>
+    <t>Plot# 31, Road# 53
+Gulshan North C.A, Gulshan-2, Dhaka-1212</t>
+  </si>
+  <si>
+    <t>Transcom Limited</t>
+  </si>
+  <si>
+    <t>https://www.symphony-mobile.com/</t>
+  </si>
+  <si>
+    <t>Rangs Babylonia
+Level 6 - 9, 246 Bir Uttam Mir Shawkat Road, Tejgaon I/A, Dhaka-1208</t>
+  </si>
+  <si>
+    <t>880 2 8878057</t>
+  </si>
+  <si>
+    <t>https://www.symphony-mobile.com/contact-us.php</t>
+  </si>
+  <si>
+    <t>Symphony Mobile</t>
+  </si>
+  <si>
+    <t>https://www.waltonbd.com/</t>
+  </si>
+  <si>
+    <t>Plot-1088, Block-I, Sabrina Sobhan Road
+    P.O-Khilkhet, P.S-Vatara,
+    Bashundhara R/A, Dhaka-1229</t>
+  </si>
+  <si>
+    <t>info@waltonbd.com</t>
+  </si>
+  <si>
+    <t>008809606-555555</t>
+  </si>
+  <si>
+    <t>Walton Group</t>
+  </si>
+  <si>
+    <t>Microsoft Bangladesh Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laila Tower, 4th Floor
+8 Gulshan Avenue, Gulshan - 1
+Dhaka 1212
+Bangladesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">880-2-8832973-75 </t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/contact_bn-bd.aspx</t>
+  </si>
+  <si>
+    <t>https://www.otobi.com/</t>
+  </si>
+  <si>
+    <t>Plot 12, Block CWS (C)
+Gulshan South Avenue, Gulshan 1,Dhaka 1212, Bangladesh.</t>
+  </si>
+  <si>
+    <t>880 2-9863219-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@otobi.com </t>
+  </si>
+  <si>
+    <t>OTOBI LIMITED</t>
   </si>
 </sst>
 </file>
@@ -158,7 +723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -176,6 +741,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -458,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +1053,7 @@
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="45.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -573,6 +1156,625 @@
       </c>
       <c r="E6" s="4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="9">
+        <v>88028826716</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1404055220</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9609667788</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="6">
+        <v>58153970</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="6">
+        <v>8000161271</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="6">
+        <v>58813126</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>8801311</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="1">
+        <v>9560099</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" t="s">
+        <v>175</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D40">
+        <v>1755558845</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D41" t="s">
+        <v>183</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D42" t="s">
+        <v>189</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="D43" t="s">
+        <v>193</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D44" t="s">
+        <v>197</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -587,8 +1789,71 @@
     <hyperlink ref="C6" r:id="rId8"/>
     <hyperlink ref="E5" r:id="rId9"/>
     <hyperlink ref="C5" r:id="rId10"/>
+    <hyperlink ref="E7" r:id="rId11"/>
+    <hyperlink ref="E8" r:id="rId12"/>
+    <hyperlink ref="C9" r:id="rId13"/>
+    <hyperlink ref="E9" r:id="rId14"/>
+    <hyperlink ref="C10" r:id="rId15"/>
+    <hyperlink ref="E10" r:id="rId16"/>
+    <hyperlink ref="C11" r:id="rId17"/>
+    <hyperlink ref="E11" r:id="rId18"/>
+    <hyperlink ref="E12" r:id="rId19"/>
+    <hyperlink ref="C12" r:id="rId20"/>
+    <hyperlink ref="E13" r:id="rId21"/>
+    <hyperlink ref="E14" r:id="rId22"/>
+    <hyperlink ref="C14" r:id="rId23"/>
+    <hyperlink ref="C15" r:id="rId24"/>
+    <hyperlink ref="E15" r:id="rId25"/>
+    <hyperlink ref="E16" r:id="rId26"/>
+    <hyperlink ref="C16" r:id="rId27"/>
+    <hyperlink ref="E17" r:id="rId28"/>
+    <hyperlink ref="E18" r:id="rId29"/>
+    <hyperlink ref="C19" r:id="rId30"/>
+    <hyperlink ref="E20" r:id="rId31"/>
+    <hyperlink ref="C20" r:id="rId32"/>
+    <hyperlink ref="C21" r:id="rId33"/>
+    <hyperlink ref="E21" r:id="rId34"/>
+    <hyperlink ref="C22" r:id="rId35"/>
+    <hyperlink ref="E22" r:id="rId36"/>
+    <hyperlink ref="E23" r:id="rId37"/>
+    <hyperlink ref="C24" r:id="rId38"/>
+    <hyperlink ref="E24" r:id="rId39"/>
+    <hyperlink ref="C25" r:id="rId40"/>
+    <hyperlink ref="E25" r:id="rId41"/>
+    <hyperlink ref="E26" r:id="rId42"/>
+    <hyperlink ref="C26" r:id="rId43"/>
+    <hyperlink ref="E27" r:id="rId44"/>
+    <hyperlink ref="C28" r:id="rId45"/>
+    <hyperlink ref="E28" r:id="rId46"/>
+    <hyperlink ref="C29" r:id="rId47"/>
+    <hyperlink ref="E29" r:id="rId48"/>
+    <hyperlink ref="C30" r:id="rId49"/>
+    <hyperlink ref="E30" r:id="rId50"/>
+    <hyperlink ref="E31" r:id="rId51"/>
+    <hyperlink ref="C31" r:id="rId52"/>
+    <hyperlink ref="E32" r:id="rId53"/>
+    <hyperlink ref="C32" r:id="rId54"/>
+    <hyperlink ref="C33" r:id="rId55"/>
+    <hyperlink ref="E34" r:id="rId56"/>
+    <hyperlink ref="C34" r:id="rId57"/>
+    <hyperlink ref="E35" r:id="rId58"/>
+    <hyperlink ref="C35" r:id="rId59"/>
+    <hyperlink ref="E36" r:id="rId60"/>
+    <hyperlink ref="C37" r:id="rId61"/>
+    <hyperlink ref="C39" r:id="rId62"/>
+    <hyperlink ref="E39" r:id="rId63"/>
+    <hyperlink ref="E40" r:id="rId64"/>
+    <hyperlink ref="C40" r:id="rId65"/>
+    <hyperlink ref="E41" r:id="rId66"/>
+    <hyperlink ref="C41" r:id="rId67"/>
+    <hyperlink ref="E42" r:id="rId68"/>
+    <hyperlink ref="C42" r:id="rId69"/>
+    <hyperlink ref="A42" r:id="rId70" display="https://en.wikipedia.org/wiki/Walton_Group"/>
+    <hyperlink ref="E43" r:id="rId71"/>
+    <hyperlink ref="E44" r:id="rId72"/>
+    <hyperlink ref="C44" r:id="rId73"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId74"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhancement #24 : Collected 100 company details
</commit_message>
<xml_diff>
--- a/Project Code/Data/List_of_NSU_graduates/Company Details.xlsx
+++ b/Project Code/Data/List_of_NSU_graduates/Company Details.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="442">
   <si>
     <t>Company Name</t>
   </si>
@@ -672,12 +672,789 @@
   <si>
     <t>OTOBI LIMITED</t>
   </si>
+  <si>
+    <t>Abul Khair Group (AKG</t>
+  </si>
+  <si>
+    <t>http://www.abulkhairsteel.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Plot # 15, Block #, CEN (A Baridhara Lake Trail West Side, Dhaka 1212</t>
+  </si>
+  <si>
+    <t>02-8881221</t>
+  </si>
+  <si>
+    <t>SK Corporation</t>
+  </si>
+  <si>
+    <t>01713-003817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skcorporation12@gmail.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">309,Al-Amin
+Complex,Nawab-bari Road,
+Bogra-5800, Bangladesh. </t>
+  </si>
+  <si>
+    <t>https://skcorporation.webs.com</t>
+  </si>
+  <si>
+    <t>(+8802) 9893536</t>
+  </si>
+  <si>
+    <t>ccm.bd@siemens.com</t>
+  </si>
+  <si>
+    <t>http://www.siemens.com.bd</t>
+  </si>
+  <si>
+    <t>Siemens Bangladesh</t>
+  </si>
+  <si>
+    <t>Ananda Group</t>
+  </si>
+  <si>
+    <t>LafargeHolcim Bangladesh Ltd</t>
+  </si>
+  <si>
+    <t>www.lafargeholcim.com.bd/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NinaKabbo , Level-7, 227/A , Bir Uttam Mir Shawkat Sarak,(Tejgaon gulshan Link Road) , Tejgaon, Dhaka -1208, Bangladesh</t>
+  </si>
+  <si>
+    <t>880(2)9881002-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info.ca@lafargeholcim.com </t>
+  </si>
+  <si>
+    <t>Symphony, Plot No - SE(F) 9, Road No - 142 (6th Floor)
+Gulshan Avenue (South), Dhaka - 1212</t>
+  </si>
+  <si>
+    <t>info@heidelbergcementbd.com</t>
+  </si>
+  <si>
+    <t>88-02-58811691</t>
+  </si>
+  <si>
+    <t>https://www.heidelbergcementbd.com</t>
+  </si>
+  <si>
+    <t>HeidelbergCement Bangladesh Limited</t>
+  </si>
+  <si>
+    <t>The Hongkong and Shanghai Banking Corporation Limited, Bangladesh (HSBC Bangladesh).</t>
+  </si>
+  <si>
+    <t>Level 4, Shanta Western Tower
+186 Bir Uttam Mir Shawkat Ali Road
+Tejgaon Industrial Area, Dhaka 1208</t>
+  </si>
+  <si>
+    <t>www.hsbc.com.bd</t>
+  </si>
+  <si>
+    <t>880 966 633 1000</t>
+  </si>
+  <si>
+    <t>contact@hsbc.com.bd</t>
+  </si>
+  <si>
+    <t>Land View Commercial Center (10th Floor)
+28 Gulshan North C/A, Gulshan Circle 2
+Dhaka 1212, Bangladesh</t>
+  </si>
+  <si>
+    <t>880-2-58815319</t>
+  </si>
+  <si>
+    <t>http://www.beol-bd.com</t>
+  </si>
+  <si>
+    <t>Bangladesh Edible Oil Limited (BEOL)</t>
+  </si>
+  <si>
+    <t>https://mail.beol-bd.com/owa/</t>
+  </si>
+  <si>
+    <t>http://www.kafcobd.com/</t>
+  </si>
+  <si>
+    <t>IDB Bhaban (13th Floor)
+E/8-A, Rokeya Sharani
+Sher-e-Bangla Nagar
+Dhaka 1207
+Bangladesh</t>
+  </si>
+  <si>
+    <t>880 (2) 918 3141</t>
+  </si>
+  <si>
+    <t>KARNAPHULI FERTILZER COMPANY LIMITED</t>
+  </si>
+  <si>
+    <t>https://bsrm.com/</t>
+  </si>
+  <si>
+    <t>Ali Mansion
+1207/1099 Sadarghat Road
+Chittagong, Bangladesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">880 31 2854901-10 </t>
+  </si>
+  <si>
+    <t>mail@bsrm.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BSRM Limited</t>
+  </si>
+  <si>
+    <t>https://www.rangsgroup.com/</t>
+  </si>
+  <si>
+    <t>117/A, Rangs Bhaban, Old Airport Road, Bijoy Sharani, Tejgaon, Dhaka-1215, Bangladesh.</t>
+  </si>
+  <si>
+    <t>88 02 9136743</t>
+  </si>
+  <si>
+    <t>RANGS GROUP</t>
+  </si>
+  <si>
+    <t>https://www.rangsgroup.com/contact/</t>
+  </si>
+  <si>
+    <t>T. K. Bhaban (2nd Floor),
+13, Karwan Bazar,
+Dhaka-1215,
+Bangladesh.</t>
+  </si>
+  <si>
+    <t>880-2-9115210</t>
+  </si>
+  <si>
+    <t>info@tkgroupbd.com</t>
+  </si>
+  <si>
+    <t>http://www.tkgroupbd.net</t>
+  </si>
+  <si>
+    <t>T. K. Group of Industries</t>
+  </si>
+  <si>
+    <t>Rahimafrooz (Bangladesh) Ltd.</t>
+  </si>
+  <si>
+    <t>Arzed Chamber
+13 Mohakhali C/A, Dhaka 1212</t>
+  </si>
+  <si>
+    <t>9893442-3</t>
+  </si>
+  <si>
+    <t>http://www.rahimafrooz.com</t>
+  </si>
+  <si>
+    <t>http://bpc.gov.bd/</t>
+  </si>
+  <si>
+    <t>http://jamunaoil.gov.bd/</t>
+  </si>
+  <si>
+    <t>http://pocl.gov.bd/</t>
+  </si>
+  <si>
+    <t>Padma Oil Company Limited</t>
+  </si>
+  <si>
+    <t>Padma Bhaban,Strand Road
+Chattogram, Bangladesh</t>
+  </si>
+  <si>
+    <t>88 031 614235-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> info@pocl.gov.bd</t>
+  </si>
+  <si>
+    <t>BTMC Bhaban, 10th Floor, 7-9 Karwan Bazar, Dhaka.</t>
+  </si>
+  <si>
+    <t>Bangladesh Petroleum Corporation</t>
+  </si>
+  <si>
+    <t>02-8189558</t>
+  </si>
+  <si>
+    <t>https://www.titasgas.org.bd</t>
+  </si>
+  <si>
+    <t>Titas Gas Transmission &amp; Distribution Company Limited</t>
+  </si>
+  <si>
+    <t>Zakir Complex, H No: K-218, Kuril Chou rasta, Progoti Sharani, Dhaka-1219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phoenix Tower (Level 8)
+117, Tejgaon Industrial Area
+Dhaka- 1208 </t>
+  </si>
+  <si>
+    <t>http://rankstelecom.com</t>
+  </si>
+  <si>
+    <t>customercare@rankstelecom.net</t>
+  </si>
+  <si>
+    <t>Ranks Telecom Limited</t>
+  </si>
+  <si>
+    <t>PETROCENTRE, 3 KAWRAN BAZAR C/A,
+DHAKA-1215, BANGLADESH</t>
+  </si>
+  <si>
+    <t>880 2 8189944</t>
+  </si>
+  <si>
+    <t>info@petrobangla.org.bd</t>
+  </si>
+  <si>
+    <t>PETROBANGLA</t>
+  </si>
+  <si>
+    <t>https://petrobangla.org.bd/</t>
+  </si>
+  <si>
+    <t>http://www.uabdl.com/</t>
+  </si>
+  <si>
+    <t>House # 7, Dolon Chapa (2nd floor), Road # 12, Sector # 1,
+Uttara Model Town, Dhaka-1230 Bangladesh.</t>
+  </si>
+  <si>
+    <t>info@uabdl.com</t>
+  </si>
+  <si>
+    <t>880 2 8932338</t>
+  </si>
+  <si>
+    <t>https://www.flynovoair.com/</t>
+  </si>
+  <si>
+    <t>United Airways BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">House-50, Road-11, Block-F, Banani. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">88-09666722224 </t>
+  </si>
+  <si>
+    <t>info@flynovoair.com</t>
+  </si>
+  <si>
+    <t>NOVOAIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA Tower (Level-5), Plot#1, Road#134, Block SE(A), Gulshan-1, Dhaka 1212 </t>
+  </si>
+  <si>
+    <t>sales.gulshan@flyregent.com</t>
+  </si>
+  <si>
+    <t>http://www.flyregent.com</t>
+  </si>
+  <si>
+    <t>Regent Airways</t>
+  </si>
+  <si>
+    <t>https://usbair.com/</t>
+  </si>
+  <si>
+    <t>77, Sohrawardi Avenue, Baridhara Diplomatic Zone
+Dhaka - 1212, Bangladesh.</t>
+  </si>
+  <si>
+    <t>info@usbair.com</t>
+  </si>
+  <si>
+    <t>US-Bangla Airlines</t>
+  </si>
+  <si>
+    <t>http://www.hameemgroup.net/</t>
+  </si>
+  <si>
+    <t>Ha-Meem Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">387, Tejgaon Industrial Area
+Dhaka-1208, Bangladesh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">880-2-8170593 </t>
+  </si>
+  <si>
+    <t>delwar@hameemgroup.com</t>
+  </si>
+  <si>
+    <t>https://renata-ltd.com/</t>
+  </si>
+  <si>
+    <t>Plot No. 1, Milk Vita Road, Section-7,
+Mirpur, Dhaka-1216, Bangladesh,
+GPO Box No. 303</t>
+  </si>
+  <si>
+    <t>8001450-54</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> info@renata-ltd.com</t>
+  </si>
+  <si>
+    <t>Renata Limited,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Trade Center, Level 6,
+08 Panthapath, Karwan Bazar, Dhaka-1215, Bangladesh. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> info@cg-bd.com</t>
+  </si>
+  <si>
+    <t>880-9102543,</t>
+  </si>
+  <si>
+    <t>Confidence Group</t>
+  </si>
+  <si>
+    <t>https://www.confidencegroup.com.bd</t>
+  </si>
+  <si>
+    <t>http://www.opsonin-pharma.com</t>
+  </si>
+  <si>
+    <t>http://www.inceptapharma.com/</t>
+  </si>
+  <si>
+    <t>40 Shahid Tajuddin Ahmed Sarani
+Tejgaon I/A, Dhaka-1208. Bangladesh</t>
+  </si>
+  <si>
+    <t>88 02) 8891688 - 703</t>
+  </si>
+  <si>
+    <t>Incepta Pharmaceuticals Ltd.</t>
+  </si>
+  <si>
+    <t>info@inceptapharma.com</t>
+  </si>
+  <si>
+    <t>Opsonin Building, 30, New Eskaton Road
+Dkhaka 1000, Bangladesh.</t>
+  </si>
+  <si>
+    <t>880-2-9332262</t>
+  </si>
+  <si>
+    <t>info@opsonin-pharma.com</t>
+  </si>
+  <si>
+    <t>Opsonin Pharma. A</t>
+  </si>
+  <si>
+    <t>Eskayef Pharmaceuticals Ltd.</t>
+  </si>
+  <si>
+    <t>http://www.skfbd.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pharmacovigilance.query@skf.transcombd.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gulshan Tower
+Plot No. 31 Road No. 53
+Gulshan North C/A
+Dhaka-1212, Bangladesh. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8818327, 8814662 </t>
+  </si>
+  <si>
+    <t>RUPAYAN CENTRE (3rd, 4th, 5th, 7th, 9th, 13th, 14th, 17th, 18th, 21st Floor), 72, Mohakhali, C/A, Dhaka-1212</t>
+  </si>
+  <si>
+    <t>02 9862573</t>
+  </si>
+  <si>
+    <t>info@rupayangroup.com</t>
+  </si>
+  <si>
+    <t>www.rupayangroup.com</t>
+  </si>
+  <si>
+    <t>Rupayan Group</t>
+  </si>
+  <si>
+    <t>59/B, Kemal Ataturk Avenue, Banani, Dhaka-1213.</t>
+  </si>
+  <si>
+    <t>info@easternhousing.com</t>
+  </si>
+  <si>
+    <t>www.easternhousing.com</t>
+  </si>
+  <si>
+    <t>Eastern Housing Ltd.</t>
+  </si>
+  <si>
+    <t>Biman Bangladesh Airlines LTD.
+Head Office, "BALAKA", Kurmitola, Dhaka-1229, Bangladesh</t>
+  </si>
+  <si>
+    <t>88-02-8901500-22</t>
+  </si>
+  <si>
+    <t>dgmgs@bdbiman.com</t>
+  </si>
+  <si>
+    <t>https://www.biman-airlines.com</t>
+  </si>
+  <si>
+    <t>Biman Bangladesh Airlines Ltd.</t>
+  </si>
+  <si>
+    <t>ACI Centre, 245 Tejgaon Industrial Area, Dhaka 1208.</t>
+  </si>
+  <si>
+    <t>info@acimotors-bd.com</t>
+  </si>
+  <si>
+    <t>ACI Motors Limited</t>
+  </si>
+  <si>
+    <t>https://acimotors-bd.com</t>
+  </si>
+  <si>
+    <t>http://www.kohinoor-bd.com</t>
+  </si>
+  <si>
+    <t>Orion House, 153-154, Tejgaon I/A,
+Dhaka -1208, Bangladesh.</t>
+  </si>
+  <si>
+    <t>KOHINOOR CHEMICAL CO. (BD) LTD</t>
+  </si>
+  <si>
+    <t>880-2-8891267-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmed Kazi Tower, House-35, Road-02, Dhanmondi, Dhaka-1205 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> info@kazifarms.com</t>
+  </si>
+  <si>
+    <t>http://www.kazifarms.com</t>
+  </si>
+  <si>
+    <t>Kazi Farms Group™</t>
+  </si>
+  <si>
+    <t>http://www.partexproperties.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    House 14, Road 3, Block I,
+    Banani, Dhaka</t>
+  </si>
+  <si>
+    <t>017.5560.7330</t>
+  </si>
+  <si>
+    <t>properties@partex.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Partex Properties
+</t>
+  </si>
+  <si>
+    <t>House# 01, Road# 04, Dhanmondi, Dhaka 1205</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Labaid Group.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  info@labaidgroup.com</t>
+  </si>
+  <si>
+    <t>www.labaidgroup.com</t>
+  </si>
+  <si>
+    <t>88 02 58610793-8</t>
+  </si>
+  <si>
+    <t>Delta Life Tower (3rd &amp; 6th floor), Plot # 37 Rd No 90, Dhaka 1212</t>
+  </si>
+  <si>
+    <t>Crown Cement Group (CCG)</t>
+  </si>
+  <si>
+    <t>https://crowncement.com</t>
+  </si>
+  <si>
+    <t>info@crowncement.com</t>
+  </si>
+  <si>
+    <t>01730709005,</t>
+  </si>
+  <si>
+    <t>http://www.shohagh.biz/</t>
+  </si>
+  <si>
+    <t>Shohag Group</t>
+  </si>
+  <si>
+    <t>63 Malibagh,DIT Road,Shahid Faruk Taslim Sarak; 1217 Dhaka, Bangladesh</t>
+  </si>
+  <si>
+    <t>http://www.btcl.com.bd/en</t>
+  </si>
+  <si>
+    <t>Telejogajog Bhaban, 37/E, Eskaton Garden
+Dkaka-1000, Bangladesh.</t>
+  </si>
+  <si>
+    <t>ddt@btcl.net.bd</t>
+  </si>
+  <si>
+    <t>9320080-3</t>
+  </si>
+  <si>
+    <t>Bangladesh Telecommunications Company Ltd. (BTCL)</t>
+  </si>
+  <si>
+    <t>http://www.daffodil-bd.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64/3 Lake Circus, Kalabagan
+Mirpur Road, Dhaka 1205, Bangladesh </t>
+  </si>
+  <si>
+    <t>8802 9116600</t>
+  </si>
+  <si>
+    <t>secretary@daffodil-bd.com</t>
+  </si>
+  <si>
+    <t>Daffodil Computers Ltd</t>
+  </si>
+  <si>
+    <t>Navana Furniture, Head Office</t>
+  </si>
+  <si>
+    <t>House # 16/B, Road # 93, Gulshan 2, Dhaka 1212</t>
+  </si>
+  <si>
+    <t>info@navanafurniture.com.com</t>
+  </si>
+  <si>
+    <t>http://www.navanafurniture.com</t>
+  </si>
+  <si>
+    <t>http://www.beximcosynthetics.com/</t>
+  </si>
+  <si>
+    <t>Kabirpur, Savar, Dhaka
+Bangladesh</t>
+  </si>
+  <si>
+    <t>88 02 7701168-70</t>
+  </si>
+  <si>
+    <t>Beximco Synthetics Ltd.</t>
+  </si>
+  <si>
+    <t>https://www.akijcement.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info.akijcement@akij.net
+</t>
+  </si>
+  <si>
+    <t>198 Bir Uttam Mir Shawkat Sarak Gulshan Link Road, Tejgaon, Dhaka-1208</t>
+  </si>
+  <si>
+    <t>Akij Group</t>
+  </si>
+  <si>
+    <t>Plot-33, section 7, Mirpur.
+Dhaka-1216, Bangladesh.</t>
+  </si>
+  <si>
+    <t>88 02 9004405</t>
+  </si>
+  <si>
+    <t>info@argondenims.com</t>
+  </si>
+  <si>
+    <t>http://www.argondenims.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argon Denims Ltd. </t>
+  </si>
+  <si>
+    <t>PriyoPrangon
+House- 19, Road 17, 6th floor
+Kamal Atarurk Avenue, Banani , Dhaka</t>
+  </si>
+  <si>
+    <t>880-2-9897734</t>
+  </si>
+  <si>
+    <t>http://www.keyagroupbd.com</t>
+  </si>
+  <si>
+    <t>kgroup@keya-bd.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keya Group </t>
+  </si>
+  <si>
+    <t>House # 17, Road # 6, Sector # 1,Uttara Model Town, Dhaka 1230, Bangladesh</t>
+  </si>
+  <si>
+    <t>8802 8933612</t>
+  </si>
+  <si>
+    <t>info@maksonsgroup.com.bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Maksons Group</t>
+  </si>
+  <si>
+    <t>http://www.maksonsgroup.com.bd</t>
+  </si>
+  <si>
+    <t>http://www.linde.com.bd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Linde Group </t>
+  </si>
+  <si>
+    <t>285 Tejgaon Industrial Area
+Dhaka – 1208
+Bangladesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">880.2.8870322-27 </t>
+  </si>
+  <si>
+    <t>info.bd@linde.com</t>
+  </si>
+  <si>
+    <t>C.P. BANGLADESH CO., LTD</t>
+  </si>
+  <si>
+    <t>Holding No : E-236, Ward No : 007, Chandra, Kaliakoir, Gazipur</t>
+  </si>
+  <si>
+    <t>info@cpbangladesh.com</t>
+  </si>
+  <si>
+    <t>http://www.cpbangladesh.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAOWA Complex (Level 7-8), VIP Road, Mohakhali, Dhaka -1206, Bangladesh </t>
+  </si>
+  <si>
+    <t>bgdinfo@care.org</t>
+  </si>
+  <si>
+    <t>http://www.carebangladesh.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARE Bangladesh </t>
+  </si>
+  <si>
+    <t>https://www.hyperion-bd.com/</t>
+  </si>
+  <si>
+    <t>88 01613 174174</t>
+  </si>
+  <si>
+    <t>info@hyperion-bd.com</t>
+  </si>
+  <si>
+    <t>Hyperion Builders Ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+House:02, Road:04, Block:A, Section:10,
+Mirpur, Dhaka-1216, Bangladesh</t>
+  </si>
+  <si>
+    <t>http://www.assuregroupbd.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANANDA GROUP  </t>
+  </si>
+  <si>
+    <t>10/1 (9th Floor), City Heart, 
+67 Nayapaltan, Dhaka – 1000, Bangladesh</t>
+  </si>
+  <si>
+    <t>www.anandagroup.com</t>
+  </si>
+  <si>
+    <t>http://www.habibgroupbd.com/</t>
+  </si>
+  <si>
+    <t>HG Tower , 1182 Jubilee Road ,
+Chittagong, Bangladesh</t>
+  </si>
+  <si>
+    <t>88-031-2868204-7,2868841-3</t>
+  </si>
+  <si>
+    <t>Habib Group</t>
+  </si>
+  <si>
+    <t>Aarong</t>
+  </si>
+  <si>
+    <t>B, Link Road, 346 Bijoy Sarani - Tejgaon Link Rd, Dhaka 1208</t>
+  </si>
+  <si>
+    <t>02-8891418</t>
+  </si>
+  <si>
+    <t>https://www.aarong.com/</t>
+  </si>
+  <si>
+    <t>https://www.ananta.com.bd/</t>
+  </si>
+  <si>
+    <t>Dhaka Corporate OfficeHouse 2, Road 10, Sector 11, UttaraDhaka 1230,</t>
+  </si>
+  <si>
+    <t>info@ananta.com.bd</t>
+  </si>
+  <si>
+    <t>Ananta Companies</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +1474,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -723,7 +1508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -760,6 +1545,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1041,10 +1828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,6 +2579,877 @@
       </c>
       <c r="E45" s="5" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" t="s">
+        <v>203</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D47" t="s">
+        <v>205</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D50" t="s">
+        <v>217</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D51" t="s">
+        <v>221</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D52" t="s">
+        <v>227</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D53" t="s">
+        <v>230</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="D54" t="s">
+        <v>236</v>
+      </c>
+      <c r="E54" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D55" t="s">
+        <v>240</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D56" t="s">
+        <v>245</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D57" t="s">
+        <v>249</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D58" t="s">
+        <v>255</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D59" t="s">
+        <v>266</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C61" t="s">
+        <v>263</v>
+      </c>
+      <c r="D61" t="s">
+        <v>262</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D62">
+        <v>1939921137</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D63">
+        <v>9617112233</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D64" t="s">
+        <v>275</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D65" t="s">
+        <v>282</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D66" t="s">
+        <v>286</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D67">
+        <v>8801730358840</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D68">
+        <v>9884818</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C69" t="s">
+        <v>301</v>
+      </c>
+      <c r="D69" t="s">
+        <v>300</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>306</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C70" t="s">
+        <v>305</v>
+      </c>
+      <c r="D70" t="s">
+        <v>304</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C71" t="s">
+        <v>308</v>
+      </c>
+      <c r="D71" t="s">
+        <v>309</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="D72" t="s">
+        <v>319</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D73" t="s">
+        <v>315</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D74" t="s">
+        <v>326</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="D75" t="s">
+        <v>328</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D76">
+        <v>55033669</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D77" t="s">
+        <v>337</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="D79" t="s">
+        <v>348</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C80" t="s">
+        <v>350</v>
+      </c>
+      <c r="D80">
+        <v>9612184</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D81" t="s">
+        <v>355</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C82" t="s">
+        <v>360</v>
+      </c>
+      <c r="D82" t="s">
+        <v>362</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D83" t="s">
+        <v>367</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="D85" t="s">
+        <v>374</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D86" t="s">
+        <v>378</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>381</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="C87" t="s">
+        <v>383</v>
+      </c>
+      <c r="D87">
+        <v>1713156840</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="D88" t="s">
+        <v>387</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="D89" s="8">
+        <v>8801711555061</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="D90" t="s">
+        <v>394</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D92" t="s">
+        <v>404</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="D93" t="s">
+        <v>411</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D95">
+        <v>9889122</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="D96" t="s">
+        <v>422</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E97" s="4" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="D98">
+        <v>9331510</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="D99" t="s">
+        <v>432</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="D100" t="s">
+        <v>436</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="D101">
+        <v>1713199799</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -1871,8 +3529,98 @@
     <hyperlink ref="C44" r:id="rId73"/>
     <hyperlink ref="C45" r:id="rId74"/>
     <hyperlink ref="E45" r:id="rId75"/>
+    <hyperlink ref="E46" r:id="rId76"/>
+    <hyperlink ref="C47" r:id="rId77"/>
+    <hyperlink ref="E47" r:id="rId78"/>
+    <hyperlink ref="C48" r:id="rId79"/>
+    <hyperlink ref="E48" r:id="rId80"/>
+    <hyperlink ref="E50" r:id="rId81"/>
+    <hyperlink ref="C50" r:id="rId82"/>
+    <hyperlink ref="C51" r:id="rId83"/>
+    <hyperlink ref="E51" r:id="rId84"/>
+    <hyperlink ref="E52" r:id="rId85"/>
+    <hyperlink ref="C52" r:id="rId86"/>
+    <hyperlink ref="E53" r:id="rId87"/>
+    <hyperlink ref="C53" r:id="rId88"/>
+    <hyperlink ref="E55" r:id="rId89"/>
+    <hyperlink ref="C55" r:id="rId90"/>
+    <hyperlink ref="E56" r:id="rId91"/>
+    <hyperlink ref="C56" r:id="rId92"/>
+    <hyperlink ref="C57" r:id="rId93"/>
+    <hyperlink ref="E57" r:id="rId94"/>
+    <hyperlink ref="E58" r:id="rId95"/>
+    <hyperlink ref="E59" r:id="rId96"/>
+    <hyperlink ref="E60" r:id="rId97"/>
+    <hyperlink ref="E61" r:id="rId98"/>
+    <hyperlink ref="E62" r:id="rId99"/>
+    <hyperlink ref="E63" r:id="rId100"/>
+    <hyperlink ref="C63" r:id="rId101"/>
+    <hyperlink ref="C64" r:id="rId102"/>
+    <hyperlink ref="E64" r:id="rId103"/>
+    <hyperlink ref="E65" r:id="rId104"/>
+    <hyperlink ref="C65" r:id="rId105"/>
+    <hyperlink ref="E66" r:id="rId106"/>
+    <hyperlink ref="C66" r:id="rId107"/>
+    <hyperlink ref="C67" r:id="rId108"/>
+    <hyperlink ref="E67" r:id="rId109"/>
+    <hyperlink ref="E68" r:id="rId110"/>
+    <hyperlink ref="C68" r:id="rId111"/>
+    <hyperlink ref="E69" r:id="rId112"/>
+    <hyperlink ref="E70" r:id="rId113"/>
+    <hyperlink ref="E71" r:id="rId114"/>
+    <hyperlink ref="E72" r:id="rId115"/>
+    <hyperlink ref="E73" r:id="rId116"/>
+    <hyperlink ref="C73" r:id="rId117"/>
+    <hyperlink ref="C72" r:id="rId118"/>
+    <hyperlink ref="E74" r:id="rId119"/>
+    <hyperlink ref="C74" r:id="rId120"/>
+    <hyperlink ref="C75" r:id="rId121"/>
+    <hyperlink ref="E75" r:id="rId122"/>
+    <hyperlink ref="C76" r:id="rId123"/>
+    <hyperlink ref="E76" r:id="rId124"/>
+    <hyperlink ref="A77" r:id="rId125" display="https://www.biman-airlines.com/"/>
+    <hyperlink ref="C77" r:id="rId126"/>
+    <hyperlink ref="E77" r:id="rId127"/>
+    <hyperlink ref="C78" r:id="rId128"/>
+    <hyperlink ref="E78" r:id="rId129"/>
+    <hyperlink ref="E79" r:id="rId130"/>
+    <hyperlink ref="E80" r:id="rId131"/>
+    <hyperlink ref="C81" r:id="rId132"/>
+    <hyperlink ref="E81" r:id="rId133"/>
+    <hyperlink ref="E82" r:id="rId134"/>
+    <hyperlink ref="E83" r:id="rId135"/>
+    <hyperlink ref="C83" r:id="rId136"/>
+    <hyperlink ref="E84" r:id="rId137"/>
+    <hyperlink ref="E85" r:id="rId138"/>
+    <hyperlink ref="C85" r:id="rId139"/>
+    <hyperlink ref="E86" r:id="rId140"/>
+    <hyperlink ref="C86" r:id="rId141"/>
+    <hyperlink ref="E87" r:id="rId142"/>
+    <hyperlink ref="E88" r:id="rId143"/>
+    <hyperlink ref="E89" r:id="rId144"/>
+    <hyperlink ref="C89" r:id="rId145"/>
+    <hyperlink ref="C90" r:id="rId146"/>
+    <hyperlink ref="E90" r:id="rId147"/>
+    <hyperlink ref="E91" r:id="rId148"/>
+    <hyperlink ref="C91" r:id="rId149"/>
+    <hyperlink ref="C92" r:id="rId150"/>
+    <hyperlink ref="E92" r:id="rId151"/>
+    <hyperlink ref="E93" r:id="rId152"/>
+    <hyperlink ref="C93" r:id="rId153"/>
+    <hyperlink ref="C94" r:id="rId154"/>
+    <hyperlink ref="E94" r:id="rId155"/>
+    <hyperlink ref="C95" r:id="rId156"/>
+    <hyperlink ref="E95" r:id="rId157"/>
+    <hyperlink ref="E96" r:id="rId158"/>
+    <hyperlink ref="C96" r:id="rId159"/>
+    <hyperlink ref="E97" r:id="rId160"/>
+    <hyperlink ref="E98" r:id="rId161"/>
+    <hyperlink ref="E99" r:id="rId162"/>
+    <hyperlink ref="E100" r:id="rId163"/>
+    <hyperlink ref="E101" r:id="rId164"/>
+    <hyperlink ref="C101" r:id="rId165"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId76"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId166"/>
 </worksheet>
 </file>
</xml_diff>